<commit_message>
Implement reading scalars from non-index Excel
Reading from old style non-index Excel files now works as well.
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -8,26 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22E66A6-C159-FC4F-82F7-49627A94B5E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32240549-A7BC-AB4C-9CBC-34DE586FA45D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
-    <sheet name="indus89Scalars" sheetId="2" r:id="rId2"/>
-    <sheet name="specialValues" sheetId="4" r:id="rId3"/>
-    <sheet name="colMerge" sheetId="5" r:id="rId4"/>
-    <sheet name="cMerge" sheetId="6" r:id="rId5"/>
-    <sheet name="merge_clear" sheetId="7" r:id="rId6"/>
-    <sheet name="skippingRC" sheetId="8" r:id="rId7"/>
-    <sheet name="ignoringRC" sheetId="9" r:id="rId8"/>
-    <sheet name="vareqIndex" sheetId="15" r:id="rId9"/>
-    <sheet name="vareq" sheetId="14" r:id="rId10"/>
-    <sheet name="indexErrors" sheetId="17" r:id="rId11"/>
-    <sheet name="testIndex" sheetId="10" r:id="rId12"/>
-    <sheet name="readingSets" sheetId="12" r:id="rId13"/>
-    <sheet name="index" sheetId="11" r:id="rId14"/>
-    <sheet name="scalarIndex" sheetId="13" r:id="rId15"/>
+    <sheet name="i11" sheetId="19" r:id="rId2"/>
+    <sheet name="drc" sheetId="18" r:id="rId3"/>
+    <sheet name="indus89Scalars" sheetId="2" r:id="rId4"/>
+    <sheet name="specialValues" sheetId="4" r:id="rId5"/>
+    <sheet name="colMerge" sheetId="5" r:id="rId6"/>
+    <sheet name="cMerge" sheetId="6" r:id="rId7"/>
+    <sheet name="merge_clear" sheetId="7" r:id="rId8"/>
+    <sheet name="repco" sheetId="20" r:id="rId9"/>
+    <sheet name="skippingRC" sheetId="8" r:id="rId10"/>
+    <sheet name="ignoringRC" sheetId="9" r:id="rId11"/>
+    <sheet name="vareqIndex" sheetId="15" r:id="rId12"/>
+    <sheet name="vareq" sheetId="14" r:id="rId13"/>
+    <sheet name="indexErrors" sheetId="17" r:id="rId14"/>
+    <sheet name="testIndex" sheetId="10" r:id="rId15"/>
+    <sheet name="readingSets" sheetId="12" r:id="rId16"/>
+    <sheet name="index" sheetId="11" r:id="rId17"/>
+    <sheet name="scalarIndex" sheetId="13" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="245">
   <si>
     <t>a</t>
   </si>
@@ -762,6 +765,18 @@
   </si>
   <si>
     <t>the1</t>
+  </si>
+  <si>
+    <t>uni1</t>
+  </si>
+  <si>
+    <t>uni2</t>
+  </si>
+  <si>
+    <t>uni3</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -1235,6 +1250,378 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30762238-98DA-45CE-9761-025334B11F1E}">
+  <dimension ref="A2:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="7">
+        <v>5000</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6000</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2200</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C06FB40-2428-4461-91B5-C67F9F6CDF6A}">
+  <dimension ref="C1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="9">
+        <v>9999</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>9999</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="9">
+        <v>9999</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>9999</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="9">
+        <v>9999</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9999</v>
+      </c>
+      <c r="G6" s="9">
+        <v>9999</v>
+      </c>
+      <c r="H6" s="9">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="9">
+        <v>9999</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="8">
+        <v>34</v>
+      </c>
+      <c r="G7" s="9">
+        <v>9999</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="9">
+        <v>9999</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="9">
+        <v>9999</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B86B91-F6DD-9F48-BB6D-2D0CD9E55B37}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767AA967-FC47-454C-82EE-900F7302B414}">
   <dimension ref="A1:P20"/>
   <sheetViews>
@@ -1580,7 +1967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FBC7DD-B3DA-1F48-BB86-AB3A6EB6257C}">
   <dimension ref="A1:M30"/>
   <sheetViews>
@@ -2007,12 +2394,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2531,7 +2918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D100155A-0898-49D0-A115-F1FA0B4B7B47}">
   <dimension ref="A1:F60"/>
   <sheetViews>
@@ -3150,7 +3537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
   <dimension ref="A1:M34"/>
   <sheetViews>
@@ -3820,12 +4207,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
   <dimension ref="C12:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3852,33 +4239,33 @@
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
-        <v>203</v>
+        <v>25</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="8">
-        <v>1</v>
-      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C14" s="8" t="s">
-        <v>25</v>
+        <v>203</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="8"/>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C15" s="8" t="s">
@@ -3903,14 +4290,6 @@
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C17" s="8"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C18" s="8"/>
@@ -4076,11 +4455,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC195D2-95BD-B743-B85D-B10B6B12EB84}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E4A174-9E1B-F040-8747-415909C9A3CD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4347,7 +4827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7AB797-14E2-4D4A-84E4-C1610623069B}">
   <dimension ref="A1:S10"/>
   <sheetViews>
@@ -4502,7 +4982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE40B61-BE36-4D1F-B26D-EE1B8ECBDED6}">
   <dimension ref="B2:F5"/>
   <sheetViews>
@@ -4571,7 +5051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D23E35-61E0-4776-924C-26830D62F350}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -4658,7 +5138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91017A3B-5F50-4354-A551-93DA6E261CE3}">
   <dimension ref="B1:N12"/>
   <sheetViews>
@@ -4804,372 +5284,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30762238-98DA-45CE-9761-025334B11F1E}">
-  <dimension ref="A2:F7"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4B60D9-EB84-C544-9828-090CE7E47B2C}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="7">
-        <v>5000</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="7">
-        <v>6000</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2200</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2000</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C06FB40-2428-4461-91B5-C67F9F6CDF6A}">
-  <dimension ref="C1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="9">
-        <v>9999</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9">
-        <v>9999</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="9">
-        <v>9999</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="8">
-        <v>2</v>
-      </c>
-      <c r="G5" s="9">
-        <v>9999</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="9">
-        <v>9999</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="9">
-        <v>9999</v>
-      </c>
-      <c r="G6" s="9">
-        <v>9999</v>
-      </c>
-      <c r="H6" s="9">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="9">
-        <v>9999</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="8">
-        <v>34</v>
-      </c>
-      <c r="G7" s="9">
-        <v>9999</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="9">
-        <v>9999</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="8">
-        <v>5</v>
-      </c>
-      <c r="G8" s="9">
-        <v>9999</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B86B91-F6DD-9F48-BB6D-2D0CD9E55B37}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>10000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add tests for documentation example and CL args
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32240549-A7BC-AB4C-9CBC-34DE586FA45D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802665F4-982D-AF4F-8C6B-E6176ABFEDB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="4" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="250">
   <si>
     <t>a</t>
   </si>
@@ -777,6 +777,21 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>_gmsopt_solver</t>
+  </si>
+  <si>
+    <t>CBC</t>
+  </si>
+  <si>
+    <t>indus89Scalars!AA4</t>
+  </si>
+  <si>
+    <t>ayayay</t>
+  </si>
+  <si>
+    <t>CPLEX</t>
   </si>
 </sst>
 </file>
@@ -4211,11 +4226,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
   <dimension ref="C12:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="12" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C12" s="10" t="s">
@@ -4290,6 +4308,14 @@
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C18" s="8"/>
@@ -4541,7 +4567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E4A174-9E1B-F040-8747-415909C9A3CD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4557,15 +4583,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -4573,7 +4599,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4581,7 +4607,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4589,15 +4615,18 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AA4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4605,7 +4634,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4622,7 +4651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -4639,7 +4668,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -4656,7 +4685,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -4673,7 +4702,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -4690,7 +4719,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -4707,24 +4736,24 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12">
         <v>0.5</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>240</v>
+      <c r="I12" t="s">
+        <v>245</v>
       </c>
       <c r="J12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+      <c r="K12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -4732,16 +4761,16 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="J13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K13" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -4749,24 +4778,33 @@
         <v>0.8</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K14" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
xlsio: Ignore value cells when detecting empty records
When detecting empty records to skip during Excel import, we now ignore the value column. This is consistent with the GDXXRW behaviour. (closes #285)
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802665F4-982D-AF4F-8C6B-E6176ABFEDB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0990B0A4-E976-0C4A-8D0F-24CCEB8EB93D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="4" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="254">
   <si>
     <t>a</t>
   </si>
@@ -792,6 +792,18 @@
   </si>
   <si>
     <t>CPLEX</t>
+  </si>
+  <si>
+    <t>modedistancea</t>
+  </si>
+  <si>
+    <t>readingSets!N23</t>
+  </si>
+  <si>
+    <t>i9a</t>
+  </si>
+  <si>
+    <t>readingSets!Q36</t>
   </si>
 </sst>
 </file>
@@ -2413,7 +2425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C35" sqref="C35:F38"/>
     </sheetView>
   </sheetViews>
@@ -2935,10 +2947,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D100155A-0898-49D0-A115-F1FA0B4B7B47}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3111,7 +3123,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>167</v>
       </c>
@@ -3139,7 +3151,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>83</v>
@@ -3152,7 +3164,7 @@
       </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>80</v>
       </c>
@@ -3167,7 +3179,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>82</v>
       </c>
@@ -3182,7 +3194,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>109</v>
       </c>
@@ -3196,8 +3208,32 @@
         <v>1500</v>
       </c>
       <c r="E23" s="10"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N24" s="10"/>
+      <c r="O24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>169</v>
       </c>
@@ -3207,8 +3243,23 @@
         <v>124</v>
       </c>
       <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O25" s="10">
+        <v>100</v>
+      </c>
+      <c r="P25" s="10">
+        <v>6000</v>
+      </c>
+      <c r="Q25" s="10">
+        <v>0</v>
+      </c>
+      <c r="R25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
         <v>80</v>
@@ -3222,8 +3273,23 @@
       <c r="E26" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="O26" s="10">
+        <v>200</v>
+      </c>
+      <c r="P26" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>2200</v>
+      </c>
+      <c r="R26" s="10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
         <v>83</v>
@@ -3237,8 +3303,21 @@
       <c r="E27" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N27" s="10"/>
+      <c r="O27" s="10">
+        <v>0</v>
+      </c>
+      <c r="P27" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>2200</v>
+      </c>
+      <c r="R27" s="10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>77</v>
       </c>
@@ -3254,8 +3333,23 @@
       <c r="E28" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N28" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="O28" s="10">
+        <v>0</v>
+      </c>
+      <c r="P28" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="10">
+        <v>2800</v>
+      </c>
+      <c r="R28" s="10">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>79</v>
       </c>
@@ -3272,7 +3366,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>76</v>
       </c>
@@ -3289,7 +3383,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>125</v>
       </c>
@@ -3306,79 +3400,147 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>170</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B34" s="10"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="Q36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="R36" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S36" s="10">
+        <v>6000</v>
+      </c>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="10"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="Q37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="R37" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="S37" s="10">
+        <v>0</v>
+      </c>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q38" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="R38" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S38" s="10">
+        <v>0</v>
+      </c>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>172</v>
       </c>
       <c r="B39" s="10"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="Q39" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="R39" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="S39" s="10">
+        <v>0</v>
+      </c>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>173</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="R40" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>174</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="R41" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>175</v>
       </c>
       <c r="B42" s="10"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="R42" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>176</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="R43" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>177</v>
       </c>
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>88</v>
       </c>
@@ -3386,7 +3548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>90</v>
       </c>
@@ -3394,7 +3556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>92</v>
       </c>
@@ -3554,15 +3716,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -3848,22 +4010,22 @@
       <c r="F16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="H17" s="7" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="H17" s="10" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3872,41 +4034,35 @@
         <v>129</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>146</v>
+        <v>252</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7">
-        <v>2</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="H18" s="7" t="s">
-        <v>184</v>
-      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D19" s="7">
-        <v>1</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="D19" s="7"/>
       <c r="E19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
-      <c r="K19">
-        <v>0</v>
+      <c r="H19" s="7" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -3914,27 +4070,30 @@
         <v>147</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
       </c>
       <c r="E20" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>162</v>
@@ -3949,25 +4108,26 @@
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10">
+      <c r="A22" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
         <v>2</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10" t="s">
-        <v>184</v>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
+      <c r="K22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -3975,7 +4135,7 @@
         <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>162</v>
@@ -3988,16 +4148,13 @@
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>162</v>
@@ -4006,16 +4163,12 @@
         <v>1</v>
       </c>
       <c r="E24" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="8"/>
-      <c r="I24">
-        <v>27</v>
-      </c>
-      <c r="J24" t="s">
-        <v>194</v>
+      <c r="H24" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -4023,68 +4176,76 @@
         <v>129</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="D25" s="10"/>
+        <v>162</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
       <c r="E25" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="10"/>
-      <c r="K25">
-        <v>0</v>
+      <c r="G25" s="10"/>
+      <c r="H25" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="D26" s="10">
-        <v>3</v>
-      </c>
-      <c r="E26" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
       <c r="F26" s="10"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="8"/>
+      <c r="I26">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>200</v>
+        <v>137</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D27" s="10">
-        <v>3</v>
-      </c>
-      <c r="E27" s="10"/>
+        <v>153</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10">
+        <v>1</v>
+      </c>
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="H27" s="10"/>
+      <c r="K27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>201</v>
+      <c r="B28" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>199</v>
@@ -4092,16 +4253,16 @@
       <c r="D28" s="10">
         <v>3</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>190</v>
-      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>202</v>
+      <c r="B29" s="10" t="s">
+        <v>200</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>199</v>
@@ -4109,19 +4270,22 @@
       <c r="D29" s="10">
         <v>3</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="11" t="s">
-        <v>182</v>
-      </c>
+      <c r="H29" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>199</v>
@@ -4129,72 +4293,62 @@
       <c r="D30" s="10">
         <v>3</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="10" t="s">
-        <v>184</v>
+      <c r="H30" s="11" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="10">
+        <v>3</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="10">
+        <v>3</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B33" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="10">
-        <v>1</v>
-      </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="10">
-        <v>1</v>
-      </c>
-      <c r="E33" s="10">
-        <v>1</v>
-      </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="M33" t="s">
-        <v>178</v>
+      <c r="E33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4202,18 +4356,65 @@
         <v>147</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10">
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10">
         <v>2</v>
       </c>
-      <c r="K34">
+      <c r="K36">
         <v>0</v>
       </c>
     </row>
@@ -4226,7 +4427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
   <dimension ref="C12:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Symbol names from Excel layout now case-insensitive
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0990B0A4-E976-0C4A-8D0F-24CCEB8EB93D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E595BD9-0EDF-A442-8DFC-36C35CA84971}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -491,9 +491,6 @@
     <t>distance</t>
   </si>
   <si>
-    <t>modedistance</t>
-  </si>
-  <si>
     <t>testIndex!A2:C2</t>
   </si>
   <si>
@@ -804,6 +801,9 @@
   </si>
   <si>
     <t>readingSets!Q36</t>
+  </si>
+  <si>
+    <t>Modedistance</t>
   </si>
 </sst>
 </file>
@@ -824,6 +824,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1550,10 +1551,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>126</v>
@@ -1565,18 +1566,18 @@
         <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10">
@@ -1589,10 +1590,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10">
@@ -1603,15 +1604,15 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>227</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>228</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10">
@@ -1622,10 +1623,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>231</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="D5" s="11">
         <v>2</v>
@@ -1633,10 +1634,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1660,36 +1661,36 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" t="s">
         <v>220</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>221</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>222</v>
       </c>
-      <c r="E1" t="s">
-        <v>223</v>
-      </c>
       <c r="L1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M1" t="s">
+        <v>219</v>
+      </c>
+      <c r="N1" t="s">
         <v>220</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>221</v>
       </c>
-      <c r="O1" t="s">
-        <v>222</v>
-      </c>
       <c r="P1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>2.56778</v>
@@ -1698,7 +1699,7 @@
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1707,7 +1708,7 @@
         <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L2">
         <v>123</v>
@@ -1722,12 +1723,12 @@
         <v>66</v>
       </c>
       <c r="P2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1736,7 +1737,7 @@
         <v>200.23</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1744,7 +1745,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4">
         <v>1.2345600000000001</v>
@@ -1753,7 +1754,7 @@
         <v>-1.234</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1768,10 +1769,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G9" s="8">
         <v>2.56778</v>
@@ -1781,10 +1782,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G10" s="8">
         <v>100</v>
@@ -1794,10 +1795,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E11" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
@@ -1807,69 +1808,69 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L12" t="s">
+        <v>228</v>
+      </c>
+      <c r="M12" t="s">
+        <v>228</v>
+      </c>
+      <c r="N12" t="s">
+        <v>228</v>
+      </c>
+      <c r="O12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P12" t="s">
         <v>229</v>
-      </c>
-      <c r="M12" t="s">
-        <v>229</v>
-      </c>
-      <c r="N12" t="s">
-        <v>229</v>
-      </c>
-      <c r="O12" t="s">
-        <v>229</v>
-      </c>
-      <c r="P12" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E13" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="N13" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="O13" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="O13" s="8" t="s">
-        <v>223</v>
-      </c>
       <c r="P13" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E14" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G14">
         <v>200.23</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L14" s="8">
         <v>2.56778</v>
@@ -1878,7 +1879,7 @@
         <v>100</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O14" s="8">
         <v>1</v>
@@ -1889,16 +1890,16 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E15" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L15" s="8">
         <v>0</v>
@@ -1907,7 +1908,7 @@
         <v>200.23</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O15" s="8">
         <v>2</v>
@@ -1918,16 +1919,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E16" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K16" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="G16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="L16" s="8">
         <v>1.2345600000000001</v>
@@ -1936,7 +1937,7 @@
         <v>-1.234</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O16" s="8">
         <v>0</v>
@@ -1947,10 +1948,10 @@
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E17" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G17" s="8">
         <v>1.2345600000000001</v>
@@ -1958,10 +1959,10 @@
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E18" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G18" s="8">
         <v>-1.234</v>
@@ -1969,10 +1970,10 @@
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E19" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1980,13 +1981,13 @@
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E20" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2019,10 +2020,10 @@
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -2033,7 +2034,7 @@
         <v>130</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10">
@@ -2054,7 +2055,7 @@
         <v>132</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -2127,10 +2128,10 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>126</v>
@@ -2153,7 +2154,7 @@
         <v>130</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10">
@@ -2174,7 +2175,7 @@
         <v>132</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -2214,10 +2215,10 @@
       <c r="F14" s="10"/>
       <c r="G14" s="8"/>
       <c r="H14" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>126</v>
@@ -2238,7 +2239,7 @@
         <v>130</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10">
@@ -2257,7 +2258,7 @@
         <v>130</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -2898,7 +2899,7 @@
         <v>83</v>
       </c>
       <c r="F35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
@@ -2923,7 +2924,7 @@
         <v>83</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.2">
@@ -2949,7 +2950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D100155A-0898-49D0-A115-F1FA0B4B7B47}">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+    <sheetView topLeftCell="F22" workbookViewId="0">
       <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
@@ -2957,7 +2958,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3021,7 +3022,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -3058,14 +3059,14 @@
         <v>114</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3142,13 +3143,13 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -3235,7 +3236,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -3402,13 +3403,13 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="10"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B34" s="10"/>
       <c r="Q34" s="10"/>
@@ -3477,7 +3478,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="10"/>
       <c r="Q39" s="10" t="s">
@@ -3494,7 +3495,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>79</v>
@@ -3505,7 +3506,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>125</v>
@@ -3516,7 +3517,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B42" s="10"/>
       <c r="R42" s="10" t="s">
@@ -3525,7 +3526,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>76</v>
@@ -3536,7 +3537,7 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B45" s="10"/>
     </row>
@@ -3561,7 +3562,7 @@
         <v>92</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -3586,7 +3587,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -3676,7 +3677,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -3718,8 +3719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3745,19 +3746,19 @@
         <v>128</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3768,7 +3769,7 @@
         <v>130</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7">
@@ -3785,7 +3786,7 @@
         <v>132</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -3802,7 +3803,7 @@
         <v>133</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7">
@@ -3810,7 +3811,7 @@
       </c>
       <c r="F4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3821,7 +3822,7 @@
         <v>134</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7">
@@ -3829,7 +3830,7 @@
       </c>
       <c r="F5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -3840,7 +3841,7 @@
         <v>135</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7">
@@ -3854,10 +3855,10 @@
         <v>129</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7">
@@ -3883,7 +3884,7 @@
         <v>138</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7">
@@ -3912,7 +3913,7 @@
         <v>139</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7">
@@ -3920,7 +3921,7 @@
       </c>
       <c r="F11" s="7"/>
       <c r="H11" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3931,7 +3932,7 @@
         <v>140</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7">
@@ -3948,7 +3949,7 @@
         <v>141</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7">
@@ -3965,7 +3966,7 @@
         <v>142</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
@@ -3984,7 +3985,7 @@
         <v>143</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7">
@@ -4001,7 +4002,7 @@
         <v>144</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7">
@@ -4018,7 +4019,7 @@
         <v>145</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10">
@@ -4026,7 +4027,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -4034,10 +4035,10 @@
         <v>129</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>253</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
@@ -4054,7 +4055,7 @@
         <v>146</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7">
@@ -4062,7 +4063,7 @@
       </c>
       <c r="F19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -4073,7 +4074,7 @@
         <v>148</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
@@ -4093,10 +4094,10 @@
         <v>147</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>149</v>
+        <v>253</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D21" s="10">
         <v>1</v>
@@ -4112,10 +4113,10 @@
         <v>147</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="D22" s="7">
         <v>1</v>
@@ -4135,10 +4136,10 @@
         <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D23" s="10">
         <v>1</v>
@@ -4154,10 +4155,10 @@
         <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="10">
         <v>1</v>
@@ -4168,7 +4169,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -4176,10 +4177,10 @@
         <v>129</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D25" s="10">
         <v>1</v>
@@ -4190,7 +4191,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -4198,10 +4199,10 @@
         <v>147</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" s="10">
         <v>1</v>
@@ -4216,7 +4217,7 @@
         <v>27</v>
       </c>
       <c r="J26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -4227,7 +4228,7 @@
         <v>137</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10">
@@ -4245,10 +4246,10 @@
         <v>129</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>199</v>
       </c>
       <c r="D28" s="10">
         <v>3</v>
@@ -4262,10 +4263,10 @@
         <v>129</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D29" s="10">
         <v>3</v>
@@ -4274,7 +4275,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="8"/>
       <c r="H29" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -4285,16 +4286,16 @@
         <v>129</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D30" s="10">
         <v>3</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -4302,10 +4303,10 @@
         <v>129</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" s="10">
         <v>3</v>
@@ -4314,7 +4315,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -4322,10 +4323,10 @@
         <v>129</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" s="10">
         <v>3</v>
@@ -4334,7 +4335,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4342,10 +4343,10 @@
         <v>147</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>206</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -4356,10 +4357,10 @@
         <v>147</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D34" s="10">
         <v>1</v>
@@ -4378,10 +4379,10 @@
         <v>147</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D35" s="10">
         <v>1</v>
@@ -4395,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -4403,10 +4404,10 @@
         <v>147</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D36" s="10">
         <v>1</v>
@@ -4438,10 +4439,10 @@
   <sheetData>
     <row r="12" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C12" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>126</v>
@@ -4453,7 +4454,7 @@
         <v>128</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.2">
@@ -4461,7 +4462,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -4472,10 +4473,10 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C14" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10">
@@ -4488,10 +4489,10 @@
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C15" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10">
@@ -4505,17 +4506,17 @@
         <v>31</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
@@ -4550,10 +4551,10 @@
       <c r="G21" s="10"/>
       <c r="H21" s="8"/>
       <c r="I21" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K21" s="10" t="s">
         <v>126</v>
@@ -4565,7 +4566,7 @@
         <v>128</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
@@ -4576,10 +4577,10 @@
       <c r="G22" s="10"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10">
@@ -4693,16 +4694,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
         <v>241</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>242</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>243</v>
-      </c>
-      <c r="D1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4716,7 +4717,7 @@
         <v>83</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4742,7 +4743,7 @@
         <v>83</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4824,7 +4825,7 @@
         <v>0.3</v>
       </c>
       <c r="AA4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -4846,7 +4847,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>21</v>
@@ -4854,7 +4855,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7">
         <v>0.6</v>
@@ -4945,13 +4946,13 @@
         <v>0.5</v>
       </c>
       <c r="I12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J12" t="s">
+        <v>247</v>
+      </c>
+      <c r="K12" t="s">
         <v>248</v>
-      </c>
-      <c r="K12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
@@ -4962,7 +4963,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
[Xlsio] Fix more issues with empty symbols
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E595BD9-0EDF-A442-8DFC-36C35CA84971}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D64B69-6D43-9E43-B3B0-9AAC2D9D732F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" tabRatio="728" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="31480" windowHeight="17200" tabRatio="728" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -29,20 +29,30 @@
     <sheet name="indexErrors" sheetId="17" r:id="rId14"/>
     <sheet name="testIndex" sheetId="10" r:id="rId15"/>
     <sheet name="readingSets" sheetId="12" r:id="rId16"/>
-    <sheet name="index" sheetId="11" r:id="rId17"/>
-    <sheet name="scalarIndex" sheetId="13" r:id="rId18"/>
+    <sheet name="emptySym" sheetId="22" r:id="rId17"/>
+    <sheet name="emptySym2" sheetId="23" r:id="rId18"/>
+    <sheet name="emptySymIndex" sheetId="21" r:id="rId19"/>
+    <sheet name="index" sheetId="11" r:id="rId20"/>
+    <sheet name="scalarIndex" sheetId="13" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="258">
   <si>
     <t>a</t>
   </si>
@@ -804,6 +814,18 @@
   </si>
   <si>
     <t>Modedistance</t>
+  </si>
+  <si>
+    <t>emptySym!A2</t>
+  </si>
+  <si>
+    <t>emptySym2!A2</t>
+  </si>
+  <si>
+    <t>emptySym2!A5</t>
+  </si>
+  <si>
+    <t>i2 </t>
   </si>
 </sst>
 </file>
@@ -2426,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:F38"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3716,708 +3738,228 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
-  <dimension ref="A1:M36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8669DA6B-1543-704C-A1BC-27666B9B4A69}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="1" max="4" width="8.83203125" style="8"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="H4" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="H5" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="L10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="H11" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="7">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>159</v>
-      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="H17" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7">
-        <v>2</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="H19" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1</v>
-      </c>
-      <c r="E20" s="7">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D21" s="10">
-        <v>1</v>
-      </c>
-      <c r="E21" s="10">
-        <v>2</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="D22" s="7">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7">
-        <v>2</v>
-      </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="10">
-        <v>1</v>
-      </c>
-      <c r="E23" s="10">
-        <v>2</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D24" s="10">
-        <v>1</v>
-      </c>
-      <c r="E24" s="10">
-        <v>2</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D25" s="10">
-        <v>1</v>
-      </c>
-      <c r="E25" s="10">
-        <v>2</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="10">
-        <v>1</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="8"/>
-      <c r="I26">
-        <v>27</v>
-      </c>
-      <c r="J26" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>152</v>
-      </c>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="10">
-        <v>1</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="10"/>
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D28" s="10">
-        <v>3</v>
-      </c>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="10">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D30" s="10">
-        <v>3</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D31" s="10">
-        <v>3</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D32" s="10">
-        <v>3</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10">
-        <v>1</v>
-      </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D35" s="10">
-        <v>1</v>
-      </c>
-      <c r="E35" s="10">
-        <v>1</v>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="M35" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="10">
-        <v>1</v>
-      </c>
-      <c r="E36" s="10">
-        <v>2</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="10"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4425,257 +3967,307 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
-  <dimension ref="C12:N33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642B7CBF-4D68-2D46-8DB1-2F8C4F105FFE}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="8.83203125" style="8"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="10"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007566C8-FB2B-E245-BB22-58F4EEE774FD}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="8"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="E12" s="10" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10">
-        <v>1</v>
-      </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10">
-        <v>0</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C18" s="8"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="8"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="L21" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="M21" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="8"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10">
-        <v>0</v>
-      </c>
-      <c r="M22" s="10"/>
-      <c r="N22" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="8"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="8"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="8"/>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="8"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="8"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="8"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="8"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="8"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="8"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="8"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4759,6 +4351,973 @@
       <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
+  <dimension ref="A1:M36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="L10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="H17" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7">
+        <v>2</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="10">
+        <v>2</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10">
+        <v>2</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1</v>
+      </c>
+      <c r="E24" s="10">
+        <v>2</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10">
+        <v>2</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="8"/>
+      <c r="I26">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10">
+        <v>1</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="10"/>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="10">
+        <v>3</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="10">
+        <v>3</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="10">
+        <v>3</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="10">
+        <v>3</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="10">
+        <v>3</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10">
+        <v>2</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
+  <dimension ref="C12:N33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C18" s="8"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C19" s="8"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C20" s="8"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C21" s="8"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C22" s="8"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10">
+        <v>0</v>
+      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C23" s="8"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C24" s="8"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C25" s="8"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C26" s="8"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C27" s="8"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="8"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C29" s="8"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Xlsio] Fix reading with multiple rdim and cdim
Reading symbols with both rdim and cdim > 1 resulted in bad data being read.
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D64B69-6D43-9E43-B3B0-9AAC2D9D732F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7C049B-16CF-A446-B236-D329FE804DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="31480" windowHeight="17200" tabRatio="728" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="260">
   <si>
     <t>a</t>
   </si>
@@ -826,6 +826,12 @@
   </si>
   <si>
     <t>i2 </t>
+  </si>
+  <si>
+    <t>modedistanceb</t>
+  </si>
+  <si>
+    <t>readingSets!N50</t>
   </si>
 </sst>
 </file>
@@ -2448,8 +2454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2972,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D100155A-0898-49D0-A115-F1FA0B4B7B47}">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView topLeftCell="F22" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3587,7 +3593,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>94</v>
       </c>
@@ -3596,7 +3602,7 @@
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>96</v>
       </c>
@@ -3606,8 +3612,19 @@
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="O50" s="10"/>
+      <c r="P50" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="S50" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>178</v>
       </c>
@@ -3615,8 +3632,19 @@
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="O51" s="10"/>
+      <c r="P51" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="S51" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
@@ -3628,8 +3656,26 @@
       <c r="E52" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N52" t="s">
+        <v>0</v>
+      </c>
+      <c r="O52" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="P52" s="10">
+        <v>100</v>
+      </c>
+      <c r="Q52" s="10">
+        <v>6000</v>
+      </c>
+      <c r="R52" s="10">
+        <v>0</v>
+      </c>
+      <c r="S52" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>80</v>
       </c>
@@ -3645,8 +3691,26 @@
       <c r="E53" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N53" t="s">
+        <v>0</v>
+      </c>
+      <c r="O53" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="P53" s="10">
+        <v>200</v>
+      </c>
+      <c r="Q53" s="10">
+        <v>0</v>
+      </c>
+      <c r="R53" s="10">
+        <v>2200</v>
+      </c>
+      <c r="S53" s="10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>80</v>
       </c>
@@ -3662,8 +3726,21 @@
       <c r="E54" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="O54" s="10"/>
+      <c r="P54" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="10">
+        <v>0</v>
+      </c>
+      <c r="R54" s="10">
+        <v>2200</v>
+      </c>
+      <c r="S54" s="10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>82</v>
       </c>
@@ -3679,8 +3756,26 @@
       <c r="E55" s="10">
         <v>2200</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="N55" t="s">
+        <v>0</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="P55" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="10">
+        <v>0</v>
+      </c>
+      <c r="R55" s="10">
+        <v>2800</v>
+      </c>
+      <c r="S55" s="10">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>82</v>
       </c>
@@ -3697,7 +3792,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>179</v>
       </c>
@@ -3706,7 +3801,7 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10" t="s">
@@ -3719,7 +3814,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10">
@@ -3741,7 +3836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8669DA6B-1543-704C-A1BC-27666B9B4A69}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4359,10 +4454,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4750,54 +4845,57 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="10">
         <v>1</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="10">
         <v>2</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="K22">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="K22" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="10">
-        <v>1</v>
-      </c>
-      <c r="E23" s="10">
+      <c r="A23" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D23" s="7">
         <v>2</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="E23" s="7">
+        <v>2</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+      <c r="K23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>161</v>
@@ -4810,16 +4908,13 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="10" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>161</v>
@@ -4832,16 +4927,16 @@
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" t="s">
-        <v>189</v>
+      <c r="H25" s="10" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>161</v>
@@ -4850,37 +4945,38 @@
         <v>1</v>
       </c>
       <c r="E26" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="8"/>
-      <c r="I26">
-        <v>27</v>
-      </c>
-      <c r="J26" t="s">
-        <v>193</v>
+      <c r="H26" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="10"/>
+        <v>161</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
       <c r="E27" s="10">
         <v>1</v>
       </c>
       <c r="F27" s="10"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="10"/>
-      <c r="K27">
-        <v>0</v>
+      <c r="G27" s="10"/>
+      <c r="H27" s="8"/>
+      <c r="I27">
+        <v>27</v>
+      </c>
+      <c r="J27" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -4888,24 +4984,28 @@
         <v>129</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>197</v>
+        <v>137</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D28" s="10">
-        <v>3</v>
-      </c>
-      <c r="E28" s="10"/>
+        <v>152</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10">
+        <v>1</v>
+      </c>
       <c r="F28" s="10"/>
       <c r="G28" s="8"/>
+      <c r="H28" s="10"/>
+      <c r="K28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>198</v>
@@ -4916,19 +5016,13 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>200</v>
+      <c r="B30" s="10" t="s">
+        <v>199</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>198</v>
@@ -4936,16 +5030,22 @@
       <c r="D30" s="10">
         <v>3</v>
       </c>
-      <c r="H30" s="11" t="s">
-        <v>189</v>
-      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>198</v>
@@ -4953,11 +5053,8 @@
       <c r="D31" s="10">
         <v>3</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
       <c r="H31" s="11" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -4965,7 +5062,7 @@
         <v>129</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>198</v>
@@ -4976,44 +5073,42 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="10" t="s">
-        <v>183</v>
+      <c r="H32" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D33" s="10">
+        <v>3</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B34" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10">
-        <v>1</v>
-      </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="K34">
-        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -5021,7 +5116,7 @@
         <v>147</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>185</v>
@@ -5037,27 +5132,49 @@
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="M35" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>147</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="D36" s="10">
         <v>1</v>
       </c>
       <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10">
         <v>2</v>
       </c>
-      <c r="K36">
+      <c r="K37">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Xlsio] Fix issues with empty sheets
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7C049B-16CF-A446-B236-D329FE804DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656FA5A3-FCC4-524D-A952-4FC80AEF47DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1000" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="readingSets" sheetId="12" r:id="rId16"/>
     <sheet name="emptySym" sheetId="22" r:id="rId17"/>
     <sheet name="emptySym2" sheetId="23" r:id="rId18"/>
-    <sheet name="emptySymIndex" sheetId="21" r:id="rId19"/>
-    <sheet name="index" sheetId="11" r:id="rId20"/>
-    <sheet name="scalarIndex" sheetId="13" r:id="rId21"/>
+    <sheet name="emptySym3" sheetId="24" r:id="rId19"/>
+    <sheet name="emptySymIndex" sheetId="21" r:id="rId20"/>
+    <sheet name="index" sheetId="11" r:id="rId21"/>
+    <sheet name="scalarIndex" sheetId="13" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="263">
   <si>
     <t>a</t>
   </si>
@@ -832,6 +833,15 @@
   </si>
   <si>
     <t>readingSets!N50</t>
+  </si>
+  <si>
+    <t>emptySym3!A2</t>
+  </si>
+  <si>
+    <t>emptySym3!A1</t>
+  </si>
+  <si>
+    <t>modedistance</t>
   </si>
 </sst>
 </file>
@@ -2454,7 +2464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -2978,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D100155A-0898-49D0-A115-F1FA0B4B7B47}">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
@@ -3836,9 +3846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8669DA6B-1543-704C-A1BC-27666B9B4A69}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4294,77 +4302,15 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007566C8-FB2B-E245-BB22-58F4EEE774FD}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815C38E9-BBDA-7843-9ACC-0736861B5DD1}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="8"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4453,10 +4399,122 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007566C8-FB2B-E245-BB22-58F4EEE774FD}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="8"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -5183,7 +5241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
   <dimension ref="C12:N33"/>
   <sheetViews>

</xml_diff>

<commit_message>
[Xlsio] Support dSet option
When reading sets from Excel, MIRO now supports reading them as domain
sets (dSets) like GDXXRW. This is only supported for one-dimensional
sets and has the following effects:
- duplicates will be ignored
- set text is ignored
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656FA5A3-FCC4-524D-A952-4FC80AEF47DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9674A205-441B-F048-A285-D9A3E9232EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1000" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="3560" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="265">
   <si>
     <t>a</t>
   </si>
@@ -529,9 +529,6 @@
     <t>testIndex!B26:E26</t>
   </si>
   <si>
-    <t>testIndex!B27:E27</t>
-  </si>
-  <si>
     <t>testIndex!B20:C20</t>
   </si>
   <si>
@@ -842,6 +839,15 @@
   </si>
   <si>
     <t>modedistance</t>
+  </si>
+  <si>
+    <t>testIndex!B27</t>
+  </si>
+  <si>
+    <t>testIndex!B20</t>
+  </si>
+  <si>
+    <t>dSetText</t>
   </si>
 </sst>
 </file>
@@ -1589,10 +1595,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>126</v>
@@ -1604,18 +1610,18 @@
         <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10">
@@ -1628,10 +1634,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10">
@@ -1642,15 +1648,15 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>226</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>227</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10">
@@ -1661,10 +1667,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>231</v>
       </c>
       <c r="D5" s="11">
         <v>2</v>
@@ -1672,10 +1678,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1699,36 +1705,36 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" t="s">
         <v>219</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>220</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>221</v>
       </c>
-      <c r="E1" t="s">
-        <v>222</v>
-      </c>
       <c r="L1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N1" t="s">
         <v>219</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>220</v>
       </c>
-      <c r="O1" t="s">
-        <v>221</v>
-      </c>
       <c r="P1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2">
         <v>2.56778</v>
@@ -1737,7 +1743,7 @@
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1746,7 +1752,7 @@
         <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L2">
         <v>123</v>
@@ -1761,12 +1767,12 @@
         <v>66</v>
       </c>
       <c r="P2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1775,7 +1781,7 @@
         <v>200.23</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1783,7 +1789,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>1.2345600000000001</v>
@@ -1792,7 +1798,7 @@
         <v>-1.234</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1807,10 +1813,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G9" s="8">
         <v>2.56778</v>
@@ -1820,10 +1826,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G10" s="8">
         <v>100</v>
@@ -1833,10 +1839,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E11" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
@@ -1846,69 +1852,69 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L12" t="s">
+        <v>227</v>
+      </c>
+      <c r="M12" t="s">
+        <v>227</v>
+      </c>
+      <c r="N12" t="s">
+        <v>227</v>
+      </c>
+      <c r="O12" t="s">
+        <v>227</v>
+      </c>
+      <c r="P12" t="s">
         <v>228</v>
-      </c>
-      <c r="M12" t="s">
-        <v>228</v>
-      </c>
-      <c r="N12" t="s">
-        <v>228</v>
-      </c>
-      <c r="O12" t="s">
-        <v>228</v>
-      </c>
-      <c r="P12" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E13" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="N13" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="O13" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="O13" s="8" t="s">
-        <v>222</v>
-      </c>
       <c r="P13" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E14" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G14">
         <v>200.23</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L14" s="8">
         <v>2.56778</v>
@@ -1917,7 +1923,7 @@
         <v>100</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O14" s="8">
         <v>1</v>
@@ -1928,16 +1934,16 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E15" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L15" s="8">
         <v>0</v>
@@ -1946,7 +1952,7 @@
         <v>200.23</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O15" s="8">
         <v>2</v>
@@ -1957,16 +1963,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E16" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G16" t="s">
+        <v>222</v>
+      </c>
+      <c r="K16" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="G16" t="s">
-        <v>223</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="L16" s="8">
         <v>1.2345600000000001</v>
@@ -1975,7 +1981,7 @@
         <v>-1.234</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O16" s="8">
         <v>0</v>
@@ -1986,10 +1992,10 @@
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E17" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G17" s="8">
         <v>1.2345600000000001</v>
@@ -1997,10 +2003,10 @@
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E18" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G18" s="8">
         <v>-1.234</v>
@@ -2008,10 +2014,10 @@
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E19" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2019,13 +2025,13 @@
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E20" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2058,10 +2064,10 @@
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -2166,10 +2172,10 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>126</v>
@@ -2253,10 +2259,10 @@
       <c r="F14" s="10"/>
       <c r="G14" s="8"/>
       <c r="H14" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>126</v>
@@ -2464,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2937,7 +2943,7 @@
         <v>83</v>
       </c>
       <c r="F35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
@@ -2962,7 +2968,7 @@
         <v>83</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.2">
@@ -2996,7 +3002,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3060,7 +3066,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -3097,14 +3103,14 @@
         <v>114</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3181,13 +3187,13 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -3274,7 +3280,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -3441,13 +3447,13 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="10"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B34" s="10"/>
       <c r="Q34" s="10"/>
@@ -3516,7 +3522,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="10"/>
       <c r="Q39" s="10" t="s">
@@ -3533,7 +3539,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>79</v>
@@ -3544,7 +3550,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>125</v>
@@ -3555,7 +3561,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="10"/>
       <c r="R42" s="10" t="s">
@@ -3564,7 +3570,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>76</v>
@@ -3575,7 +3581,7 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B45" s="10"/>
     </row>
@@ -3600,7 +3606,7 @@
         <v>92</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
@@ -3636,7 +3642,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -3804,7 +3810,7 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -4105,7 +4111,7 @@
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -4327,16 +4333,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" t="s">
         <v>240</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>241</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>242</v>
-      </c>
-      <c r="D1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4350,7 +4356,7 @@
         <v>83</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4376,7 +4382,7 @@
         <v>83</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4402,14 +4408,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007566C8-FB2B-E245-BB22-58F4EEE774FD}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="8"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -4431,7 +4438,7 @@
         <v>130</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D2" s="10">
         <v>1</v>
@@ -4447,7 +4454,7 @@
         <v>132</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D3" s="10">
         <v>1</v>
@@ -4463,7 +4470,7 @@
         <v>133</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
@@ -4479,7 +4486,7 @@
         <v>146</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
@@ -4493,10 +4500,10 @@
         <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D6" s="11">
         <v>1</v>
@@ -4512,10 +4519,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4527,7 +4534,7 @@
     <col min="10" max="10" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -4541,22 +4548,25 @@
         <v>128</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>129</v>
       </c>
@@ -4573,7 +4583,7 @@
       <c r="F2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>131</v>
       </c>
@@ -4590,7 +4600,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>129</v>
       </c>
@@ -4606,10 +4616,10 @@
       </c>
       <c r="F4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>129</v>
       </c>
@@ -4625,10 +4635,10 @@
       </c>
       <c r="F5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>129</v>
       </c>
@@ -4645,12 +4655,12 @@
       <c r="F6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>152</v>
@@ -4662,7 +4672,7 @@
       <c r="F7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -4671,7 +4681,7 @@
       <c r="F8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>129</v>
       </c>
@@ -4688,7 +4698,7 @@
       <c r="F9" s="7"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -4700,7 +4710,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>129</v>
       </c>
@@ -4708,7 +4718,7 @@
         <v>139</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>154</v>
+        <v>263</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7">
@@ -4716,10 +4726,10 @@
       </c>
       <c r="F11" s="7"/>
       <c r="H11" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>131</v>
       </c>
@@ -4736,7 +4746,7 @@
       <c r="F12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>131</v>
       </c>
@@ -4752,8 +4762,11 @@
       </c>
       <c r="F13" s="7"/>
       <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>131</v>
       </c>
@@ -4772,7 +4785,7 @@
       <c r="F14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>131</v>
       </c>
@@ -4789,7 +4802,7 @@
       <c r="F15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>131</v>
       </c>
@@ -4797,7 +4810,7 @@
         <v>144</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>158</v>
+        <v>262</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7">
@@ -4805,6 +4818,9 @@
       </c>
       <c r="F16" s="7"/>
       <c r="H16" s="7"/>
+      <c r="N16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
@@ -4814,7 +4830,7 @@
         <v>145</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10">
@@ -4822,7 +4838,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="H17" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -4830,10 +4846,10 @@
         <v>129</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
@@ -4844,13 +4860,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7">
@@ -4858,7 +4874,7 @@
       </c>
       <c r="F19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -4869,7 +4885,7 @@
         <v>148</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
@@ -4889,10 +4905,10 @@
         <v>147</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="10">
         <v>1</v>
@@ -4908,10 +4924,10 @@
         <v>147</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>249</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>250</v>
       </c>
       <c r="D22" s="10">
         <v>1</v>
@@ -4930,10 +4946,10 @@
         <v>147</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>259</v>
       </c>
       <c r="D23" s="7">
         <v>2</v>
@@ -4953,10 +4969,10 @@
         <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D24" s="10">
         <v>1</v>
@@ -4972,10 +4988,10 @@
         <v>129</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D25" s="10">
         <v>1</v>
@@ -4986,7 +5002,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -4994,10 +5010,10 @@
         <v>129</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D26" s="10">
         <v>1</v>
@@ -5008,7 +5024,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -5016,10 +5032,10 @@
         <v>147</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
@@ -5034,7 +5050,7 @@
         <v>27</v>
       </c>
       <c r="J27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -5063,10 +5079,10 @@
         <v>129</v>
       </c>
       <c r="B29" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>198</v>
       </c>
       <c r="D29" s="10">
         <v>3</v>
@@ -5080,10 +5096,10 @@
         <v>129</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D30" s="10">
         <v>3</v>
@@ -5092,7 +5108,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="8"/>
       <c r="H30" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -5103,16 +5119,16 @@
         <v>129</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="10">
         <v>3</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -5120,10 +5136,10 @@
         <v>129</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="10">
         <v>3</v>
@@ -5132,7 +5148,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -5140,10 +5156,10 @@
         <v>129</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D33" s="10">
         <v>3</v>
@@ -5152,7 +5168,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -5160,10 +5176,10 @@
         <v>147</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -5174,10 +5190,10 @@
         <v>147</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D35" s="10">
         <v>1</v>
@@ -5196,10 +5212,10 @@
         <v>147</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D36" s="10">
         <v>1</v>
@@ -5213,7 +5229,7 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -5221,10 +5237,10 @@
         <v>147</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" s="10">
         <v>1</v>
@@ -5256,10 +5272,10 @@
   <sheetData>
     <row r="12" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C12" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>126</v>
@@ -5271,7 +5287,7 @@
         <v>128</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.2">
@@ -5279,7 +5295,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -5290,10 +5306,10 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C14" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10">
@@ -5306,10 +5322,10 @@
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C15" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10">
@@ -5323,17 +5339,17 @@
         <v>31</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
@@ -5368,10 +5384,10 @@
       <c r="G21" s="10"/>
       <c r="H21" s="8"/>
       <c r="I21" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K21" s="10" t="s">
         <v>126</v>
@@ -5383,7 +5399,7 @@
         <v>128</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
@@ -5394,10 +5410,10 @@
       <c r="G22" s="10"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10">
@@ -5559,7 +5575,7 @@
         <v>0.3</v>
       </c>
       <c r="AA4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -5581,7 +5597,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>21</v>
@@ -5589,7 +5605,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>0.6</v>
@@ -5680,13 +5696,13 @@
         <v>0.5</v>
       </c>
       <c r="I12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J12" t="s">
+        <v>246</v>
+      </c>
+      <c r="K12" t="s">
         <v>247</v>
-      </c>
-      <c r="K12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
@@ -5697,7 +5713,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
[Xlsio] Fix out-of-bound read
When reading a range from a sheet that comes after the last data,
MIRO incorrectly threw an error instead of returning an empty dataset.
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656FA5A3-FCC4-524D-A952-4FC80AEF47DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566DCEC0-EBC4-D848-BA4C-A6ACB20D1A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1000" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="264">
   <si>
     <t>a</t>
   </si>
@@ -842,6 +842,9 @@
   </si>
   <si>
     <t>modedistance</t>
+  </si>
+  <si>
+    <t>emptySym2!D4</t>
   </si>
 </sst>
 </file>
@@ -4400,10 +4403,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007566C8-FB2B-E245-BB22-58F4EEE774FD}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4505,6 +4508,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4514,7 +4531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Xlsio] Fix reading index without rdim and cdim
A typo caused reading index without rdim and cdim to fail.
</commit_message>
<xml_diff>
--- a/src/tests/data/exampleData.xlsx
+++ b/src/tests/data/exampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fproske/Documents/products/miro/src/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E117208-0AA3-3E4B-BB44-119185D4F2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FC941D-1F2E-1447-9FB1-7FCFA132CFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1680" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="9" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="1680" windowWidth="28800" windowHeight="15920" tabRatio="728" firstSheet="10" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readingWithValues" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,9 @@
     <sheet name="emptySym2" sheetId="23" r:id="rId18"/>
     <sheet name="emptySym3" sheetId="24" r:id="rId19"/>
     <sheet name="emptySymIndex" sheetId="21" r:id="rId20"/>
-    <sheet name="index" sheetId="11" r:id="rId21"/>
-    <sheet name="scalarIndex" sheetId="13" r:id="rId22"/>
+    <sheet name="minimalIndex" sheetId="25" r:id="rId21"/>
+    <sheet name="index" sheetId="11" r:id="rId22"/>
+    <sheet name="scalarIndex" sheetId="13" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="266">
   <si>
     <t>a</t>
   </si>
@@ -2473,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D07AAD-8BC6-403D-BD89-479E97AFC021}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:D21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4411,8 +4412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007566C8-FB2B-E245-BB22-58F4EEE774FD}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4536,11 +4537,65 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAB2B53-5788-F94C-B676-A435A0059B81}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130F2013-4443-439F-9D3B-6214B216E2DC}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5275,7 +5330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44C50D0-66DE-DD4F-AAF8-826E83C7C5AF}">
   <dimension ref="C12:N33"/>
   <sheetViews>

</xml_diff>